<commit_message>
list of dbGaP queries
</commit_message>
<xml_diff>
--- a/data/dbgap-adv/queries.xlsx
+++ b/data/dbgap-adv/queries.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/trang/PhD/Manuscripts/cardioinformatics/data/dbgap-adv/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{40E0C5E4-71BB-CF44-8D3D-5F9F090C99E2}" xr6:coauthVersionLast="40" xr6:coauthVersionMax="40" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{CB9A6846-D968-DB44-93CA-9C86B39C40C1}" xr6:coauthVersionLast="40" xr6:coauthVersionMax="40" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="28780" yWindow="460" windowWidth="51200" windowHeight="28340" xr2:uid="{1F9EA0CE-30E4-FA46-A47F-482058E57278}"/>
   </bookViews>
@@ -28,7 +28,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="3785" uniqueCount="1000">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="3787" uniqueCount="1002">
   <si>
     <t>Query URL</t>
   </si>
@@ -3028,6 +3028,12 @@
   </si>
   <si>
     <t>ResultId</t>
+  </si>
+  <si>
+    <t>Note</t>
+  </si>
+  <si>
+    <t>Web-scraping result, there were duplicated and missing studies. Dismissed</t>
   </si>
 </sst>
 </file>
@@ -3445,10 +3451,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{5007DD7B-CF0A-5941-AFAF-0FCF0BCB69A1}">
-  <dimension ref="A1:G4"/>
+  <dimension ref="A1:H4"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="170" zoomScaleNormal="170" workbookViewId="0">
-      <selection activeCell="I10" sqref="I10"/>
+      <selection activeCell="D4" sqref="D4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="14" x14ac:dyDescent="0.15"/>
@@ -3460,7 +3466,7 @@
     <col min="6" max="16384" width="10.83203125" style="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:7" x14ac:dyDescent="0.15">
+    <row r="1" spans="1:8" x14ac:dyDescent="0.15">
       <c r="A1" s="1" t="s">
         <v>964</v>
       </c>
@@ -3482,8 +3488,11 @@
       <c r="G1" s="1" t="s">
         <v>998</v>
       </c>
-    </row>
-    <row r="2" spans="1:7" x14ac:dyDescent="0.15">
+      <c r="H1" s="1" t="s">
+        <v>1000</v>
+      </c>
+    </row>
+    <row r="2" spans="1:8" x14ac:dyDescent="0.15">
       <c r="A2" s="1">
         <v>1</v>
       </c>
@@ -3506,8 +3515,11 @@
         <f>Result_0!G1</f>
         <v>658305</v>
       </c>
-    </row>
-    <row r="3" spans="1:7" x14ac:dyDescent="0.15">
+      <c r="H2" s="1" t="s">
+        <v>1001</v>
+      </c>
+    </row>
+    <row r="3" spans="1:8" x14ac:dyDescent="0.15">
       <c r="A3" s="1">
         <v>1</v>
       </c>
@@ -3531,7 +3543,7 @@
         <v>322766</v>
       </c>
     </row>
-    <row r="4" spans="1:7" x14ac:dyDescent="0.15">
+    <row r="4" spans="1:8" x14ac:dyDescent="0.15">
       <c r="A4" s="1">
         <v>2</v>
       </c>
@@ -3565,7 +3577,7 @@
   <dimension ref="A1:G112"/>
   <sheetViews>
     <sheetView zoomScale="140" zoomScaleNormal="140" workbookViewId="0">
-      <selection activeCell="G1" sqref="G1"/>
+      <selection activeCell="A8" sqref="A8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -10795,7 +10807,9 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{35FFDBC9-556F-D24C-B1FB-960FC712CD17}">
   <dimension ref="A1:P155"/>
   <sheetViews>
-    <sheetView zoomScale="150" zoomScaleNormal="150" workbookViewId="0"/>
+    <sheetView zoomScale="150" zoomScaleNormal="150" workbookViewId="0">
+      <selection sqref="A1:P155"/>
+    </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
   <cols>

</xml_diff>